<commit_message>
Adding vocabulary and illustration
</commit_message>
<xml_diff>
--- a/metadataschemas/FAIR4FOISDatasetMetadataSchema.xlsx
+++ b/metadataschemas/FAIR4FOISDatasetMetadataSchema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luiz/Documents/GitHub/fair4fois/metadataschemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hbcesar/Documents/fair4fois/metadataschemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CC0FEF-0195-4143-8F45-7E9A8CF65A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3564078-FD3C-0B40-93AF-9CAE2FFE88F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{1FD0E56F-4622-7F4A-B90A-35A31D9FEDD4}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15920" activeTab="1" xr2:uid="{1FD0E56F-4622-7F4A-B90A-35A31D9FEDD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -927,9 +927,6 @@
     <t>https://data.jrc.ec.europa.eu/dataset/7aed1a89-c904-43ed-af0f-b024fc9cb92a</t>
   </si>
   <si>
-    <t>Irregular</t>
-  </si>
-  <si>
     <t>2019-01-01 - 2024-01-01</t>
   </si>
   <si>
@@ -961,6 +958,9 @@
   </si>
   <si>
     <t>https://www.iana.org/assignments/media-types/application/zip</t>
+  </si>
+  <si>
+    <t>Three times a year</t>
   </si>
 </sst>
 </file>
@@ -1768,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D01ED1E-E282-1747-9074-FEF158706663}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1852,7 +1852,7 @@
         <v>37</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="23">
         <v>45043</v>
@@ -1861,7 +1861,7 @@
         <v>38</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="4" t="s">
@@ -1871,10 +1871,10 @@
         <v>30</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="M3" s="3"/>
     </row>
@@ -1899,7 +1899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03C3577-6738-3145-9D80-E5F8675FAE47}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1958,51 +1958,51 @@
     </row>
     <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="22">
         <v>45043</v>
       </c>
       <c r="E3" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>44</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="22">
         <v>45030</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>50</v>
       </c>
       <c r="I4" s="20"/>
     </row>

</xml_diff>

<commit_message>
Updating vocabulary and adjusting schema templates
</commit_message>
<xml_diff>
--- a/metadataschemas/FAIR4FOISDatasetMetadataSchema.xlsx
+++ b/metadataschemas/FAIR4FOISDatasetMetadataSchema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hbcesar/Documents/fair4fois/metadataschemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luiz/Documents/GitHub/fair4fois/metadataschemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3564078-FD3C-0B40-93AF-9CAE2FFE88F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CC0FEF-0195-4143-8F45-7E9A8CF65A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15920" activeTab="1" xr2:uid="{1FD0E56F-4622-7F4A-B90A-35A31D9FEDD4}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{1FD0E56F-4622-7F4A-B90A-35A31D9FEDD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -927,6 +927,9 @@
     <t>https://data.jrc.ec.europa.eu/dataset/7aed1a89-c904-43ed-af0f-b024fc9cb92a</t>
   </si>
   <si>
+    <t>Irregular</t>
+  </si>
+  <si>
     <t>2019-01-01 - 2024-01-01</t>
   </si>
   <si>
@@ -958,9 +961,6 @@
   </si>
   <si>
     <t>https://www.iana.org/assignments/media-types/application/zip</t>
-  </si>
-  <si>
-    <t>Three times a year</t>
   </si>
 </sst>
 </file>
@@ -1768,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D01ED1E-E282-1747-9074-FEF158706663}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1852,7 +1852,7 @@
         <v>37</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E3" s="23">
         <v>45043</v>
@@ -1861,7 +1861,7 @@
         <v>38</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="4" t="s">
@@ -1871,10 +1871,10 @@
         <v>30</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M3" s="3"/>
     </row>
@@ -1899,7 +1899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03C3577-6738-3145-9D80-E5F8675FAE47}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1958,51 +1958,51 @@
     </row>
     <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" s="22">
         <v>45043</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4" s="22">
         <v>45030</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I4" s="20"/>
     </row>

</xml_diff>